<commit_message>
Created most important functions, not tested
</commit_message>
<xml_diff>
--- a/CAMPOS UTILIZADOS.xlsx
+++ b/CAMPOS UTILIZADOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus Farias\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAMSUNG\Documents\Trabalho\Freelas\WhatsApp massa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5816586A-B2FB-428D-BB65-E5AB3DF978C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4184B1-B56F-45C4-A181-19C1AB0E0DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAMPOS" sheetId="1" r:id="rId1"/>
@@ -23,25 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
-  <si>
-    <t>Código</t>
-  </si>
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Contatos</t>
-  </si>
-  <si>
-    <t>Nível</t>
-  </si>
-  <si>
-    <t>Situação</t>
-  </si>
-  <si>
-    <t>Débito</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Semente</t>
   </si>
@@ -85,24 +67,6 @@
     <t>INATIVO6</t>
   </si>
   <si>
-    <t>Total de Pontos no Período</t>
-  </si>
-  <si>
-    <t>Pontos faltantes para Bronze</t>
-  </si>
-  <si>
-    <t>Pontos faltantes para Prata</t>
-  </si>
-  <si>
-    <t>Pontos faltantes para Ouro</t>
-  </si>
-  <si>
-    <t>Pontos faltantes para Diamante</t>
-  </si>
-  <si>
-    <t>Oportunidade</t>
-  </si>
-  <si>
     <t>Parcelamento de Boleto</t>
   </si>
   <si>
@@ -146,13 +110,16 @@
   </si>
   <si>
     <t>(98) 98000-0006</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +256,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -635,8 +610,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -991,316 +968,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2">
+        <v>111111111</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2">
+        <v>5500</v>
+      </c>
+      <c r="I1" s="2">
+        <v>300</v>
+      </c>
+      <c r="J1" s="2">
+        <v>900</v>
+      </c>
+      <c r="K1" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L1" s="2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>111111111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4000</v>
+      </c>
+      <c r="I2" s="2">
+        <v>300</v>
+      </c>
+      <c r="J2" s="2">
+        <v>900</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L2" s="2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>111111111</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2100</v>
+      </c>
+      <c r="I3" s="2">
+        <v>300</v>
+      </c>
+      <c r="J3" s="2">
+        <v>900</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>111111111</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2">
+        <v>850</v>
+      </c>
+      <c r="I4" s="2">
+        <v>300</v>
+      </c>
+      <c r="J4" s="2">
+        <v>900</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L4" s="2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>111111111</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="2">
+        <v>500</v>
+      </c>
+      <c r="I5" s="2">
+        <v>300</v>
+      </c>
+      <c r="J5" s="2">
+        <v>900</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>111111111</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2">
+        <v>400</v>
+      </c>
+      <c r="I6" s="2">
+        <v>300</v>
+      </c>
+      <c r="J6" s="2">
+        <v>900</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L6" s="2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>111111111</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="2">
+        <v>250</v>
+      </c>
+      <c r="I7" s="2">
+        <v>300</v>
+      </c>
+      <c r="J7" s="2">
+        <v>900</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L7" s="2">
+        <v>5500</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>111111111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>300</v>
-      </c>
-      <c r="J2">
-        <v>900</v>
-      </c>
-      <c r="K2">
-        <v>2200</v>
-      </c>
-      <c r="L2">
-        <v>5500</v>
-      </c>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>111111111</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>300</v>
-      </c>
-      <c r="J3">
-        <v>900</v>
-      </c>
-      <c r="K3">
-        <v>2200</v>
-      </c>
-      <c r="L3">
-        <v>5500</v>
-      </c>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G9" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>111111111</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>300</v>
-      </c>
-      <c r="J4">
-        <v>900</v>
-      </c>
-      <c r="K4">
-        <v>2200</v>
-      </c>
-      <c r="L4">
-        <v>5500</v>
-      </c>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>111111111</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>300</v>
-      </c>
-      <c r="J5">
-        <v>900</v>
-      </c>
-      <c r="K5">
-        <v>2200</v>
-      </c>
-      <c r="L5">
-        <v>5500</v>
-      </c>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G11" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>111111111</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>300</v>
-      </c>
-      <c r="J6">
-        <v>900</v>
-      </c>
-      <c r="K6">
-        <v>2200</v>
-      </c>
-      <c r="L6">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>111111111</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>300</v>
-      </c>
-      <c r="J7">
-        <v>900</v>
-      </c>
-      <c r="K7">
-        <v>2200</v>
-      </c>
-      <c r="L7">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>111111111</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>300</v>
-      </c>
-      <c r="J8">
-        <v>900</v>
-      </c>
-      <c r="K8">
-        <v>2200</v>
-      </c>
-      <c r="L8">
-        <v>5500</v>
-      </c>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>